<commit_message>
Save data of 25/03/2021
</commit_message>
<xml_diff>
--- a/public/files/description.xlsx
+++ b/public/files/description.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AFRICASYS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AFRICASYS\Desktop\Africasys\laravel\eSante\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06051762-658A-48BD-AECD-FD437DCF34E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2F7D23-3EBB-4380-80F3-2299C3BBC027}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="7875" xr2:uid="{299C46B8-2A37-469B-96E7-404E95C92470}"/>
   </bookViews>
@@ -34,12 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>title</t>
-  </si>
-  <si>
-    <t>Test de xlsx 1</t>
   </si>
 </sst>
 </file>
@@ -391,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D05BA50A-973C-417B-9D09-DB8E38F27B40}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,11 +406,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>